<commit_message>
查看inRunOperationID = _OPERATION_SALE_CTLS_IDLE_ 所對應的FUNCTION
</commit_message>
<xml_diff>
--- a/SRC/FlowChart/inMENU_MenuKeyInAndGetAmount.xlsx
+++ b/SRC/FlowChart/inMENU_MenuKeyInAndGetAmount.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>inFunc_Display_LOGO  透過inGetLOGONum()，顯示不同的logo</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,12 +34,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>srEventMenuItem-&gt;inRunOperationID = _OPERATION_SALE_ICC_;
-                srEventMenuItem-&gt;inRunTRTID = _TRT_SALE_;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inMENU_MenuKeyInAndGetAmount</t>
+    <t>inMENU_MenuKeyInAndGetAmount
+整體流程為偵測到輸入1~9後設定交易類型和 inRunOperationID、&gt;inRunTRTID，以跑對應的function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>會先擋srEventMenuItem-&gt;inEventCode == '0' (/* 不接受金額第一位為0 */)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                srEventMenuItem-&gt;inRunOperationID = _OPERATION_SALE_CTLS_IDLE_;
+                srEventMenuItem-&gt;inRunTRTID = _TRT_SALE_CTLS_;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,41 +373,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>